<commit_message>
[Java Service][Smoke test]update test cases
</commit_message>
<xml_diff>
--- a/autotest/service/i18n-service/APITest/resource/master/Testdata.xlsx
+++ b/autotest/service/i18n-service/APITest/resource/master/Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\VIP\Automation\javaservice\APITestChange\resource\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDFC058-456A-41F9-892C-3669F5DD0884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13915AEA-CA7F-4B83-9455-54D327F8CBF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{77E86863-578B-49A1-B922-199B6D0E141D}"/>
   </bookViews>
@@ -41912,10 +41912,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D32865FE-F68A-4B13-B8DD-197B77279CD1}">
   <dimension ref="A1:XEN384"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A171" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="AJ179" sqref="AJ179:AJ181"/>
+      <selection pane="bottomLeft" activeCell="AI105" sqref="AI105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="25.5" customHeight="1"/>

</xml_diff>

<commit_message>
[Java service][Smoke test]update bundles
</commit_message>
<xml_diff>
--- a/autotest/service/i18n-service/APITest/resource/master/Testdata.xlsx
+++ b/autotest/service/i18n-service/APITest/resource/master/Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\VIP\Automation\javaservice\APITestChange\resource\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13915AEA-CA7F-4B83-9455-54D327F8CBF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D96046-835E-4DA3-A398-629DC8DC2B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{77E86863-578B-49A1-B922-199B6D0E141D}"/>
   </bookViews>
@@ -8591,8 +8591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418B1FC6-8D16-461A-9B61-36F1539FE050}">
   <dimension ref="A1:AK498"/>
   <sheetViews>
-    <sheetView topLeftCell="W88" workbookViewId="0">
-      <selection activeCell="AJ99" sqref="AJ99"/>
+    <sheetView topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="AI211" sqref="AI211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="59.734375" defaultRowHeight="14.4"/>
@@ -41912,10 +41912,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D32865FE-F68A-4B13-B8DD-197B77279CD1}">
   <dimension ref="A1:XEN384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="AI105" sqref="AI105"/>
+      <selection pane="bottomLeft" activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="25.5" customHeight="1"/>
@@ -44885,7 +44885,7 @@
         <v>35</v>
       </c>
       <c r="G63" s="38" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H63" t="s">
         <v>37</v>

</xml_diff>